<commit_message>
Make edu_parent2 not mandatory
</commit_message>
<xml_diff>
--- a/inst/formr/bvq-1.0.1/bvq_04_demo.xlsx
+++ b/inst/formr/bvq-1.0.1/bvq_04_demo.xlsx
@@ -1,18 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ggarciad\OneDrive - San Juan de Dios\Documentos\projects\bvq\inst\formr\bvq-1.0.1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="survey" sheetId="1" state="visible" r:id="rId3"/>
-    <sheet name="choices" sheetId="2" state="visible" r:id="rId4"/>
-    <sheet name="settings" sheetId="3" state="visible" r:id="rId5"/>
+    <sheet name="survey" sheetId="1" r:id="rId1"/>
+    <sheet name="choices" sheetId="2" r:id="rId2"/>
+    <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
+  <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="ExcelA1"/>
@@ -22,246 +26,229 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
-  <si>
-    <t xml:space="preserve">type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">label</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">class</t>
-  </si>
-  <si>
-    <t xml:space="preserve">showif</t>
-  </si>
-  <si>
-    <t xml:space="preserve">value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">block_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item_order</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="67">
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>optional</t>
+  </si>
+  <si>
+    <t>class</t>
+  </si>
+  <si>
+    <t>showif</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>block_order</t>
+  </si>
+  <si>
+    <t>item_order</t>
   </si>
   <si>
     <t xml:space="preserve">note  </t>
   </si>
   <si>
-    <t xml:space="preserve">demo_title_catalan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Informació general
+    <t>demo_title_catalan</t>
+  </si>
+  <si>
+    <t># Informació general
 A continuació us demanem algunes dades sobre la vostra situació geogràfica i perfil familiar.</t>
   </si>
   <si>
-    <t xml:space="preserve">bvq_01_log$language=="catalan"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_title_spanish</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># Información general
+    <t>bvq_01_log$language=="catalan"</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>demo_title_spanish</t>
+  </si>
+  <si>
+    <t># Información general
 A continuación os pedimos algunos datos sobre vuestra situación geográfica y perfil familiar.</t>
   </si>
   <si>
-    <t xml:space="preserve">bvq_01_log$language=="spanish"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_title_english</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># General information
+    <t>bvq_01_log$language=="spanish"</t>
+  </si>
+  <si>
+    <t>demo_title_english</t>
+  </si>
+  <si>
+    <t># General information
 Below we ask for some information about your geographical situation and family profile.</t>
   </si>
   <si>
-    <t xml:space="preserve">bvq_01_log$language=="english"</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### `r paste0(dplyr::case_when(bvq_01_log$language=="catalan" ~paste0("Sexe del bebé:"), bvq_01_log$language=="spanish" ~paste0("Sexo del bebé:"), TRUE ~ paste0("Sex of the baby:")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">left400 label_align_left answer_align_left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">text 5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_postcode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### `r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Codi postal"), bvq_01_log$language == "spanish" ~paste0("Código postal"), TRUE ~ paste0("Postcode")))`
+    <t>bvq_01_log$language=="english"</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>### `r paste0(dplyr::case_when(bvq_01_log$language=="catalan" ~paste0("Sexe del bebé:"), bvq_01_log$language=="spanish" ~paste0("Sexo del bebé:"), TRUE ~ paste0("Sex of the baby:")))`</t>
+  </si>
+  <si>
+    <t>left400 label_align_left answer_align_left</t>
+  </si>
+  <si>
+    <t>text 5</t>
+  </si>
+  <si>
+    <t>demo_postcode</t>
+  </si>
+  <si>
+    <t>### `r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Codi postal"), bvq_01_log$language == "spanish" ~paste0("Código postal"), TRUE ~ paste0("Postcode")))`
 `r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Si us plau, indica'ns el teu codi postal:"), bvq_01_log$language == "spanish" ~paste0("Por favor, indícanos tu código postal:"), TRUE ~ paste0("Please, indicate your postcode:")))`</t>
   </si>
   <si>
-    <t xml:space="preserve">answer_below_label answer_align_left</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_parent_info</t>
-  </si>
-  <si>
-    <t xml:space="preserve">### `r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Informació sobre les dues persones que més temps passen amb el/la nen/a:"), bvq_01_log$language == "spanish"~paste0("Información sobre dos personas que más tiempo pasan con el/la niño/a:"), TRUE ~ paste0("Information about the two people who spend more time with the child:")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one  demo_education1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_parent1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Nivel educatiu del/de la cuidador(a) 1:"), bvq_01_log$language == "spanish"~paste0("Nivel educativo del/de la cuidador(a) 1:"), TRUE ~ paste0("Educational level of caretaker 1:")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">select_one  demo_education2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_parent2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Nivel educatiu del/de la cuidador(a) 2:"), bvq_01_log$language == "spanish"~paste0("Nivel educativo del/de la cuidador(a) 2:"), TRUE ~ paste0("Educational level of caretaker 2:")))`</t>
+    <t>answer_below_label answer_align_left</t>
+  </si>
+  <si>
+    <t>demo_parent_info</t>
+  </si>
+  <si>
+    <t>### `r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Informació sobre les dues persones que més temps passen amb el/la nen/a:"), bvq_01_log$language == "spanish"~paste0("Información sobre dos personas que más tiempo pasan con el/la niño/a:"), TRUE ~ paste0("Information about the two people who spend more time with the child:")))`</t>
+  </si>
+  <si>
+    <t>select_one  demo_education1</t>
+  </si>
+  <si>
+    <t>demo_parent1</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Nivel educatiu del/de la cuidador(a) 1:"), bvq_01_log$language == "spanish"~paste0("Nivel educativo del/de la cuidador(a) 1:"), TRUE ~ paste0("Educational level of caretaker 1:")))`</t>
+  </si>
+  <si>
+    <t>select_one  demo_education2</t>
+  </si>
+  <si>
+    <t>demo_parent2</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Nivel educatiu del/de la cuidador(a) 2:"), bvq_01_log$language == "spanish"~paste0("Nivel educativo del/de la cuidador(a) 2:"), TRUE ~ paste0("Educational level of caretaker 2:")))`</t>
   </si>
   <si>
     <t xml:space="preserve">submit  </t>
   </si>
   <si>
-    <t xml:space="preserve">submit_demo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language=="catalan"~paste0("Següent"), bvq_01_log$language=="spanish"~paste0("Siguiente"), TRUE~paste0("Next")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">list_name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_education1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noeducation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Sense escolaritzar"), bvq_01_log$language == "spanish" ~paste0("Sin escolarizar"), TRUE ~ paste0("No education")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">primary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació primària"), bvq_01_log$language == "spanish" ~paste0("Educación primaria"), TRUE ~ paste0("Primary education")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">secondary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació Secundària Obligatoria (ESO)"), bvq_01_log$language == "spanish" ~paste0("Educación Secundaria Obligatoria (ESO)"), TRUE ~ paste0("General Certificate of Secondary Education (GCSE)")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">complementary</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Batxillerat"), bvq_01_log$language == "spanish" ~paste0("Bachillerato"), TRUE ~ paste0("Complementary education")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">vocational</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Cicles formatius"), bvq_01_log$language == "spanish" ~paste0("Ciclos formativos"), TRUE ~ paste0("Vocational training")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">university</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació universitaria"), bvq_01_log$language == "spanish" ~paste0("Educación universitaria"), TRUE ~ paste0("University degree")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">demo_education2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Femení"), bvq_01_log$language == "spanish" ~paste0("Femenno"), TRUE ~ paste0("Female")))`</t>
-  </si>
-  <si>
-    <t xml:space="preserve">item</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maximum_number_displayed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">displayed_percentage_maximum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add_percentage_points</t>
-  </si>
-  <si>
-    <t xml:space="preserve">enable_instant_validation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_after</t>
-  </si>
-  <si>
-    <t xml:space="preserve">google_file_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unlinked</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_invitation_after</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expire_invitation_grace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hide_results</t>
-  </si>
-  <si>
-    <t xml:space="preserve">use_paging</t>
+    <t>submit_demo</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language=="catalan"~paste0("Següent"), bvq_01_log$language=="spanish"~paste0("Siguiente"), TRUE~paste0("Next")))`</t>
+  </si>
+  <si>
+    <t>list_name</t>
+  </si>
+  <si>
+    <t>demo_education1</t>
+  </si>
+  <si>
+    <t>noeducation</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Sense escolaritzar"), bvq_01_log$language == "spanish" ~paste0("Sin escolarizar"), TRUE ~ paste0("No education")))`</t>
+  </si>
+  <si>
+    <t>primary</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació primària"), bvq_01_log$language == "spanish" ~paste0("Educación primaria"), TRUE ~ paste0("Primary education")))`</t>
+  </si>
+  <si>
+    <t>secondary</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació Secundària Obligatoria (ESO)"), bvq_01_log$language == "spanish" ~paste0("Educación Secundaria Obligatoria (ESO)"), TRUE ~ paste0("General Certificate of Secondary Education (GCSE)")))`</t>
+  </si>
+  <si>
+    <t>complementary</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Batxillerat"), bvq_01_log$language == "spanish" ~paste0("Bachillerato"), TRUE ~ paste0("Complementary education")))`</t>
+  </si>
+  <si>
+    <t>vocational</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Cicles formatius"), bvq_01_log$language == "spanish" ~paste0("Ciclos formativos"), TRUE ~ paste0("Vocational training")))`</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Educació universitaria"), bvq_01_log$language == "spanish" ~paste0("Educación universitaria"), TRUE ~ paste0("University degree")))`</t>
+  </si>
+  <si>
+    <t>demo_education2</t>
+  </si>
+  <si>
+    <t>`r paste0(dplyr::case_when(bvq_01_log$language == "catalan" ~paste0("Femení"), bvq_01_log$language == "spanish" ~paste0("Femenno"), TRUE ~ paste0("Female")))`</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>maximum_number_displayed</t>
+  </si>
+  <si>
+    <t>displayed_percentage_maximum</t>
+  </si>
+  <si>
+    <t>add_percentage_points</t>
+  </si>
+  <si>
+    <t>enable_instant_validation</t>
+  </si>
+  <si>
+    <t>expire_after</t>
+  </si>
+  <si>
+    <t>google_file_id</t>
+  </si>
+  <si>
+    <t>unlinked</t>
+  </si>
+  <si>
+    <t>expire_invitation_after</t>
+  </si>
+  <si>
+    <t>expire_invitation_grace</t>
+  </si>
+  <si>
+    <t>hide_results</t>
+  </si>
+  <si>
+    <t>use_paging</t>
+  </si>
+  <si>
+    <t>*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="16"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -274,7 +261,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -282,100 +269,72 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1f497d"/>
+        <a:srgbClr val="1F497D"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="eeece1"/>
+        <a:srgbClr val="EEECE1"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4f81bd"/>
+        <a:srgbClr val="4F81BD"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="c0504d"/>
+        <a:srgbClr val="C0504D"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9bbb59"/>
+        <a:srgbClr val="9BBB59"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064a2"/>
+        <a:srgbClr val="8064A2"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4bacc6"/>
+        <a:srgbClr val="4BACC6"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="f79646"/>
+        <a:srgbClr val="F79646"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000ff"/>
+        <a:srgbClr val="0000FF"/>
       </a:hlink>
       <a:folHlink>
         <a:srgbClr val="800080"/>
@@ -383,12 +342,12 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -417,7 +376,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="1"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -438,7 +397,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -489,7 +448,7 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -507,34 +466,33 @@
           <a:path path="circle">
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:I1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="20"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="60.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="21.47"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="44.16"/>
+    <col min="1" max="2" width="20" style="1" customWidth="1"/>
+    <col min="3" max="3" width="60.9140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.5" style="1" customWidth="1"/>
+    <col min="6" max="6" width="44.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:9" ht="40.5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -563,7 +521,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -573,7 +531,7 @@
       <c r="C2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="n">
+      <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="F2" s="1" t="s">
@@ -582,11 +540,11 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="I2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -596,7 +554,7 @@
       <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="1" t="n">
+      <c r="D3" s="1">
         <v>1</v>
       </c>
       <c r="F3" s="1" t="s">
@@ -605,11 +563,11 @@
       <c r="H3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="1" t="n">
+      <c r="I3" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="81" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:9" ht="60.75" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>9</v>
       </c>
@@ -619,7 +577,7 @@
       <c r="C4" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="1" t="n">
+      <c r="D4" s="1">
         <v>1</v>
       </c>
       <c r="F4" s="1" t="s">
@@ -628,11 +586,11 @@
       <c r="H4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I4" s="1" t="n">
+      <c r="I4" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="19.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -648,11 +606,11 @@
       <c r="H5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="1" t="n">
+      <c r="I5" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="344.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:9" ht="162" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>23</v>
       </c>
@@ -668,11 +626,11 @@
       <c r="H6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I6" s="1" t="n">
+      <c r="I6" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="263.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
@@ -682,17 +640,17 @@
       <c r="C7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="D7" s="1">
         <v>1</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I7" s="1" t="n">
+      <c r="I7" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="202.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>29</v>
       </c>
@@ -708,11 +666,11 @@
       <c r="H8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I8" s="1" t="n">
+      <c r="I8" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="202.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>32</v>
       </c>
@@ -722,17 +680,20 @@
       <c r="C9" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="E9" s="1" t="s">
         <v>26</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="1" t="n">
+      <c r="I9" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -745,39 +706,30 @@
       <c r="H10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="n">
+      <c r="I10" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:C1048576"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
+    <sheetView topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="30"/>
+    <col min="3" max="3" width="30" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>38</v>
       </c>
@@ -788,7 +740,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>39</v>
       </c>
@@ -799,7 +751,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>39</v>
       </c>
@@ -810,7 +762,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="202.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>39</v>
       </c>
@@ -821,7 +773,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>39</v>
       </c>
@@ -832,7 +784,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
@@ -843,7 +795,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -854,7 +806,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>52</v>
       </c>
@@ -865,7 +817,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
@@ -876,7 +828,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="202.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>52</v>
       </c>
@@ -887,7 +839,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>52</v>
       </c>
@@ -898,7 +850,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="162" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>52</v>
       </c>
@@ -909,7 +861,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="182.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>52</v>
       </c>
@@ -920,43 +872,32 @@
         <v>51</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="141.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="1" t="n">
+      <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="50" zoomScaleNormal="50" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-    </sheetView>
+    <sheetView zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20" defaultRowHeight="20.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="20" defaultRowHeight="20.25" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>54</v>
       </c>
@@ -965,89 +906,84 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B2" s="1" t="n">
+      <c r="B2" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="1">
         <v>100</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="B4" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="40.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1" t="n">
+      <c r="B5" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B8" s="1" t="n">
+      <c r="B8" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B11" s="1" t="n">
+      <c r="B11" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="20.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B12" s="1" t="n">
+      <c r="B12" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>